<commit_message>
converted to a class
</commit_message>
<xml_diff>
--- a/repository/toots.xlsx
+++ b/repository/toots.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1016,6 +1016,646 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1.118516957558131e+17</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>rawchili</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>45322.72025462963</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;[Hughes] The &lt;a href="https://channels.im/tags/Jets" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Jets&lt;/span&gt;&lt;/a&gt; and Rex Hogan have mutually agreed to part ways, sources tell @snytv. The move allows Hogan, who spent the last five seasons as the team’s assistant general manager, to explore other opportunities. &lt;a href="https://www.rawchili.com/3282610/" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class=""&gt;rawchili.com/3282610/&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;a href="https://channels.im/tags/AmericanFootballConference" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;AmericanFootballConference&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/AmericanFootballConferenceSouthDivision" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;AmericanFootballConferenceSouthDivision&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/Colts" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Colts&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/Football" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Football&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/Indiana" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Indiana&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/Indianapolis" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Indianapolis&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/IndianapolisColts" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;IndianapolisColts&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/NationalFootballLeague" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;NationalFootballLeague&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/NFL" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;NFL&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1.118516957545633e+17</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>grafana</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>45322.72020833333</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;👋 Say hello to better log navigation with TableView in &lt;a href="https://grafana.social/tags/Grafana" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Grafana&lt;/span&gt;&lt;/a&gt; 10.3!&lt;/p&gt;&lt;p&gt;Learn how Grafana's TableView improves your log analysis experience.This feature simplifies navigating dense log information with an interactive, user-friendly UI, suitable for various data sources.&lt;/p&gt;&lt;p&gt;Learn about all the new features in 10.3 here: &lt;a href="https://bit.ly/3SvahWz" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;bit.ly/3SvahWz&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1.118516956509662e+17</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>bintano</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>45322.72025721065</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Tarek El Moussa Reveals Explosive Fight with Ex-Wife Christina Hall and the End of Their Seven-Year Marriage, which Prompted him to Take a Gun to the Woods&lt;br /&gt;&lt;a href="https://bintano.com/tarek-el-moussa-reveals-explosive-fight-with-ex-wife-christina-hall-and-the-end-of-their-seven-year-marriage-which-prompted-him-to-take-a-gun-to-the-woods/?feed_id=41645&amp;amp;_unique_id=65ba8095d3f36" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;bintano.com/tarek-el-moussa-re&lt;/span&gt;&lt;span class="invisible"&gt;veals-explosive-fight-with-ex-wife-christina-hall-and-the-end-of-their-seven-year-marriage-which-prompted-him-to-take-a-gun-to-the-woods/?feed_id=41645&amp;amp;_unique_id=65ba8095d3f36&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1.118516956227416e+17</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Andy_European</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>45322.72021990741</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Conservative minister: Brexit checks ‘price you pay for being a sovereign state again’&lt;/p&gt;&lt;p&gt;Nope. It’s the price you pay for being an insular, corrupt declining state.&lt;/p&gt;&lt;p&gt;Time for &lt;a href="https://mastodon.online/tags/Scotland" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Scotland&lt;/span&gt;&lt;/a&gt;🏴󠁧󠁢󠁳󠁣󠁴󠁿 to cut loose and rejoin EU.&lt;br&gt;&lt;a href="https://apple.news/ACmGOcQjoStm-BlNKyc6m8w" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;apple.news/ACmGOcQjoStm-BlNKyc&lt;/span&gt;&lt;span class="invisible"&gt;6m8w&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1.118516955890644e+17</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>bikingjp</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>45322.72019675926</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Grizl CF に付属していたこれらのシムは何のためにありますか? &lt;a href="https://www.bikingjp.com/112270/" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class=""&gt;bikingjp.com/112270/&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt; &lt;a href="https://jforo.com/tags/Bicycle" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Bicycle&lt;/span&gt;&lt;/a&gt; &lt;a href="https://jforo.com/tags/Bicycling" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Bicycling&lt;/span&gt;&lt;/a&gt; &lt;a href="https://jforo.com/tags/Bike" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Bike&lt;/span&gt;&lt;/a&gt; &lt;a href="https://jforo.com/tags/Biking" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Biking&lt;/span&gt;&lt;/a&gt; &lt;a href="https://jforo.com/tags/CanyonBicycles" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;CanyonBicycles&lt;/span&gt;&lt;/a&gt; &lt;a href="https://jforo.com/tags/CanyonBikes" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;CanyonBikes&lt;/span&gt;&lt;/a&gt; &lt;a href="https://jforo.com/tags/Cycling" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Cycling&lt;/span&gt;&lt;/a&gt; &lt;a href="https://jforo.com/tags/%E3%82%B5%E3%82%A4%E3%82%AF%E3%83%AA%E3%83%B3%E3%82%B0" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;サイクリング&lt;/span&gt;&lt;/a&gt; &lt;a href="https://jforo.com/tags/%E8%87%AA%E8%BB%A2%E8%BB%8A" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;自転車&lt;/span&gt;&lt;/a&gt; &lt;a href="https://jforo.com/tags/%E8%87%AA%E8%BB%A2%E8%BB%8A%E3%82%B5%E3%82%A4%E3%82%AF%E3%83%AA%E3%83%B3%E3%82%B0" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;自転車サイクリング&lt;/span&gt;&lt;/a&gt; &lt;a href="https://jforo.com/tags/%E8%87%AA%E8%BB%A2%E8%BB%8A%E3%81%AB%E4%B9%97%E3%82%8B" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;自転車に乗る&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1.118516955205063e+17</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>es</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>gilbert31</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>45322.72023148148</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Una investigación de ProPublica apunta a que en 2006 la campaña de &lt;a href="https://mastodon.online/tags/AMLO" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;AMLO&lt;/span&gt;&lt;/a&gt; habría recibido 2 millones de dólares del narcotráfico a cambio de promesas de impunidad.&lt;/p&gt;&lt;p&gt;¿Dos millones de dólares costó la política de "Abrazos, no balazos"? &lt;/p&gt;&lt;p&gt;&lt;a href="https://mastodon.online/tags/NarcoPresidente" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;NarcoPresidente&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.online/tags/Mexico" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Mexico&lt;/span&gt;&lt;/a&gt; &lt;/p&gt;&lt;p&gt;&lt;a href="https://www.propublica.org/article/mexico-amlo-lopez-obrador-campaign-drug-cartels" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;propublica.org/article/mexico-&lt;/span&gt;&lt;span class="invisible"&gt;amlo-lopez-obrador-campaign-drug-cartels&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1.118517533163621e+17</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>t54r4n1</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>45322.73041666667</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;opened the lunch dialog menu (fridge) and selected &lt;br&gt;🎼 waffle peanut butter 🎵 by singing it&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1.118517533108448e+17</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>iembot_gid</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>45322.73041666667</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://masto.globaleas.org/tags/GID" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;GID&lt;/span&gt;&lt;/a&gt; issues Area Forecast Discussion (AFD) at Jan 31, 11:31 AM CST &lt;a href="https://mesonet.agron.iastate.edu/p.php?pid=202401311731-KGID-FXUS63-AFDGID" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;mesonet.agron.iastate.edu/p.ph&lt;/span&gt;&lt;span class="invisible"&gt;p?pid=202401311731-KGID-FXUS63-AFDGID&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1.118517533102457e+17</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>BobVezeau</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>45322.73042824074</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://www.nytimes.com/badges/games/v1/bee.html?d=2024-01-31&amp;amp;l=badgluy&amp;amp;p=72&amp;amp;r=Genius&amp;amp;c=55e9d87ddd206ce08bfccffbcc028096&amp;amp;smid=na-share" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;nytimes.com/badges/games/v1/be&lt;/span&gt;&lt;span class="invisible"&gt;e.html?d=2024-01-31&amp;amp;l=badgluy&amp;amp;p=72&amp;amp;r=Genius&amp;amp;c=55e9d87ddd206ce08bfccffbcc028096&amp;amp;smid=na-share&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1.118517532873297e+17</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>alper</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>45322.73034722222</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;My daughters talking about Sonic: “Amy! The only girl.”&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1.118517532207936e+17</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>UT3UMS</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>45322.73039351852</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;I'll be testing the new QRP setup of Yaesu ATAS25 and Xiegu 6100 at around 21-22 UTC&lt;/p&gt;&lt;p&gt;The plan is to spend some time on FT8 and try out the voice. At least, I plan to hear myself through websdr nearby&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1.118517532183362e+17</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>es</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>olea</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>45322.7304050926</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;\o/&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1.118517532096815e+17</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Independent</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>45322.73032407407</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Conor Benn vs Peter Dobson live stream and time: How to watch fight and when does it start? &lt;/p&gt;&lt;p&gt;Here’s all you need to know as Benn enters the ring in Las Vegas, amid his ongoing ban from boxing in the UK &lt;a href="https://press.coop/tags/press" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;press&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;a href="https://www.independent.co.uk/sport/boxing/benn-dobson-watch-online-start-time-uk-b2488239.html?utm_source=press.coop" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;independent.co.uk/sport/boxing&lt;/span&gt;&lt;span class="invisible"&gt;/benn-dobson-watch-online-start-time-uk-b2488239.html?utm_source=press.coop&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1.11851753209625e+17</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>abitofzen</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>45322.7304050926</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;"Zen is laughter, laughter Zen" - Zen proverb&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1.118517541759987e+17</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>CBSSportsGolazo</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>45322.7294675926</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Omar Khribin puts Syria right back in it. 👀&lt;/p&gt;&lt;p&gt;All level between Iran and Syria with a place in the &lt;a href="https://twitter.com/hashtag/AsianCup2023" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;AsianCup2023&lt;/span&gt;&lt;/a&gt; quarterfinals on the line. 🍿&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1.118517541668284e+17</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>es</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>RGBes</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>45322.73059149305</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Disponible «Domando al escritor, edición 2024» | El Pingüino Tolkiano  &lt;br /&gt; &lt;br /&gt;&lt;a href="https://elpinguinotolkiano.wordpress.com/2024/01/31/disponible-domando-al-escritor-edicion-2024/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;elpinguinotolkiano.wordpress.c&lt;/span&gt;&lt;span class="invisible"&gt;om/2024/01/31/disponible-domando-al-escritor-edicion-2024/&lt;/span&gt;&lt;/a&gt; &lt;br /&gt; &lt;br /&gt;&lt;a href="https://mastodon.social/tags/Draw" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;Draw&lt;/span&gt;&lt;/a&gt;, &lt;a href="https://mastodon.social/tags/LibreOffice" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;LibreOffice&lt;/span&gt;&lt;/a&gt;, &lt;a href="https://mastodon.social/tags/Math" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;Math&lt;/span&gt;&lt;/a&gt;, &lt;a href="https://mastodon.social/tags/Tipograf%C3%ADa" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;Tipografía&lt;/span&gt;&lt;/a&gt;, &lt;a href="https://mastodon.social/tags/Writer" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;Writer&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1.118517541386496e+17</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>es</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Boqueroni</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>45322.73058650463</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;El &amp;quot;Colmo&amp;quot; de un extintor...😲&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1.118517541232139e+17</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Freie_Presse</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>45322.73058410879</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Hohenstein-Ernstthal: Welche Auswirkungen haben Parteiaustritte für den Stadtrat? &lt;a href="https://www.freiepresse.de/zwickau/hohenstein-ernstthal/hohenstein-ernstthal-welche-auswirkungen-haben-parteiaustritte-fuer-den-stadtrat-artikel13229287" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;freiepresse.de/zwickau/hohenst&lt;/span&gt;&lt;span class="invisible"&gt;ein-ernstthal/hohenstein-ernstthal-welche-auswirkungen-haben-parteiaustritte-fuer-den-stadtrat-artikel13229287&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1.118517540784061e+17</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>DocAtCDI</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>45322.73057714121</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;My wife’s just told me that she’s leaving me, because of my obsession for rugby. Im gutted. I begged her for one last try!&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1.118517540613303e+17</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>ashwells</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>45322.73056712963</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Now playing on Mixfix Radio: Hard To Say I'm Sorry (feat. Peter Cetera) by Az Yet! Tune in now: &lt;a href="http://chrisduffley.com:8050/radio.mp3" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;http://&lt;/span&gt;&lt;span class="ellipsis"&gt;chrisduffley.com:8050/radio.mp&lt;/span&gt;&lt;span class="invisible"&gt;3&lt;/span&gt;&lt;/a&gt;&lt;br&gt;If you'd like to download any of the songs played, go to &lt;a href="http://chrisduffley.com:8005/public/mixfix_radio/ondemand" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;http://&lt;/span&gt;&lt;span class="ellipsis"&gt;chrisduffley.com:8005/public/m&lt;/span&gt;&lt;span class="invisible"&gt;ixfix_radio/ondemand&lt;/span&gt;&lt;/a&gt;&lt;br&gt;Thanks for listening!&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1.118517540488494e+17</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>cbssports</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>45322.67268518519</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Cavaliers vs. Pistons odds, line, spread, time: 2024 NBA picks, January 31 predictions from proven model&lt;br&gt;&lt;a href="https://www.cbssports.com/nba/news/cavaliers-vs-pistons-odds-line-spread-time-2024-nba-picks-january-31-predictions-from-proven-model/?utm_source=flipboard&amp;amp;utm_medium=activitypub" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;cbssports.com/nba/news/cavalie&lt;/span&gt;&lt;span class="invisible"&gt;rs-vs-pistons-odds-line-spread-time-2024-nba-picks-january-31-predictions-from-proven-model/?utm_source=flipboard&amp;amp;utm_medium=activitypub &lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Posted into NBA&lt;br&gt;&lt;a href="https://flipboard.com/@cbssports/nba-vtb7sfeiz?utm_source=flipboard&amp;amp;utm_medium=activitypub" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;flipboard.com/@cbssports/nba-v&lt;/span&gt;&lt;span class="invisible"&gt;tb7sfeiz?utm_source=flipboard&amp;amp;utm_medium=activitypub &lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1.118517540478059e+17</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>TheNerdyBlogger</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>45322.73057048611</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;From the &lt;a href="https://mastodon.social/tags/SciFi5" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;SciFi5&lt;/span&gt;&lt;/a&gt; Archive: Happy birthday to funny man, &lt;a href="https://mastodon.social/tags/PaulScheer" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;PaulScheer&lt;/span&gt;&lt;/a&gt;! When I wrote this last year, I determined that he probably doesn&amp;#39;t sleep based on his extensive resume. &lt;a href="https://mastodon.social/tags/StarTrekLowerDecks" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;StarTrekLowerDecks&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/ParksAndRec" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;ParksAndRec&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/nerdlyfe" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;nerdlyfe&lt;/span&gt;&lt;/a&gt; &lt;a href="https://sci-fi-5.libsyn.com/paul-scheer-january-31-1976" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;sci-fi-5.libsyn.com/paul-schee&lt;/span&gt;&lt;span class="invisible"&gt;r-january-31-1976&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1.118517540421877e+17</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Fife4Europe</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>45322.73055555556</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;The Independent: Brexit news - live: Checks make it 'easier to trade with China than France'&lt;br&gt;&lt;a href="https://www.independent.co.uk/news/uk/politics/brexit-dup-border-northern-ireland-news-b2487883.html" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;independent.co.uk/news/uk/poli&lt;/span&gt;&lt;span class="invisible"&gt;tics/brexit-dup-border-northern-ireland-news-b2487883.html&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1.118517570678968e+17</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>FatBluDragon</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>45322.73108796297</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Time to give Ferg a new hairstyle!&lt;/p&gt;&lt;p&gt;&lt;a href="https://www.twitch.tv/fatbludragon" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class=""&gt;twitch.tv/fatbludragon&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1.118517570250392e+17</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>victory</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>45322.73107638889</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;So I did a bleeding heart thing and I need help with these 5 guys I rescued&lt;br&gt;&lt;a href="https://www.gofundme.com/fab-5-needs-medical-care-forever-homes" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;gofundme.com/fab-5-needs-medic&lt;/span&gt;&lt;span class="invisible"&gt;al-care-forever-homes&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1.118517569807683e+17</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>sia</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>45322.73104166667</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Yes, yes, AI is 💩 but it does make generating fake products for a fake test store fun&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1.118517569225394e+17</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>GaySk8rMarley</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="n">
+        <v>45322.73107814815</v>
+      </c>
+      <c r="E52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>1.118517569117745e+17</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ulmfn</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="n">
+        <v>45322.73106481481</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Text updated, yet traditional &lt;a href="https://anabaptistworld.org/text-updated-yet-traditional/?utm_source=CT%20Daily%20Briefing%20Newsletter&amp;amp;utm_medium=Newsletter&amp;amp;utm_term=856909&amp;amp;utm_content=15576&amp;amp;utm_campaign=email" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;anabaptistworld.org/text-updat&lt;/span&gt;&lt;span class="invisible"&gt;ed-yet-traditional/?utm_source=CT%20Daily%20Briefing%20Newsletter&amp;amp;utm_medium=Newsletter&amp;amp;utm_term=856909&amp;amp;utm_content=15576&amp;amp;utm_campaign=email&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>